<commit_message>
Implementing dynamic update of open tables
</commit_message>
<xml_diff>
--- a/Data/UBSP -- transactions.xlsx
+++ b/Data/UBSP -- transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Portfolio-management\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Y\Portfolio management\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF17019-C7DA-4974-A6BC-C6EEF4FFF283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85EDBF5-AB92-4765-ADE2-2FFDBFEC5611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{223AE522-EB96-4B82-9D33-10D4026A92AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{223AE522-EB96-4B82-9D33-10D4026A92AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Транзакции_UBS_P" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="Restricted">[1]Портфель!$G$12</definedName>
     <definedName name="Unrestricted">[1]Портфель!$G$11</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -613,8 +613,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Портфель"/>
       <sheetName val="Портфель_2022"/>
@@ -1357,116 +1360,118 @@
   <sheetPr codeName="Sheet106"/>
   <dimension ref="A1:CU146"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BF91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CN129" sqref="CN129"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" outlineLevelRow="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.64453125" customWidth="1"/>
-    <col min="3" max="3" width="2.76171875" customWidth="1"/>
-    <col min="4" max="4" width="11.64453125" customWidth="1"/>
-    <col min="5" max="5" width="9.41015625" customWidth="1"/>
-    <col min="6" max="6" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.29296875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.703125" customWidth="1"/>
-    <col min="12" max="12" width="11.64453125" customWidth="1"/>
-    <col min="13" max="13" width="9.41015625" customWidth="1"/>
-    <col min="14" max="14" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.29296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="7" customWidth="1"/>
-    <col min="18" max="18" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="1.703125" customWidth="1"/>
-    <col min="20" max="20" width="11.64453125" customWidth="1"/>
-    <col min="21" max="21" width="9.41015625" customWidth="1"/>
-    <col min="22" max="22" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.29296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" style="1" customWidth="1"/>
     <col min="25" max="25" width="7" customWidth="1"/>
-    <col min="26" max="26" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="1.703125" customWidth="1"/>
-    <col min="28" max="28" width="11.64453125" customWidth="1"/>
-    <col min="29" max="29" width="9.41015625" customWidth="1"/>
-    <col min="30" max="30" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.29296875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="1.7109375" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" customWidth="1"/>
+    <col min="29" max="29" width="9.42578125" customWidth="1"/>
+    <col min="30" max="30" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.28515625" style="1" customWidth="1"/>
     <col min="33" max="33" width="7" customWidth="1"/>
-    <col min="34" max="34" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="1.703125" customWidth="1"/>
-    <col min="36" max="36" width="11.64453125" customWidth="1"/>
-    <col min="37" max="37" width="9.41015625" customWidth="1"/>
-    <col min="38" max="38" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.29296875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="1.7109375" customWidth="1"/>
+    <col min="36" max="36" width="11.7109375" customWidth="1"/>
+    <col min="37" max="37" width="9.42578125" customWidth="1"/>
+    <col min="38" max="38" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.28515625" style="1" customWidth="1"/>
     <col min="41" max="41" width="7" customWidth="1"/>
-    <col min="42" max="42" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="1.703125" customWidth="1"/>
-    <col min="44" max="44" width="11.64453125" customWidth="1"/>
-    <col min="45" max="45" width="9.41015625" customWidth="1"/>
-    <col min="46" max="46" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.29296875" style="1" customWidth="1"/>
+    <col min="42" max="42" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="1.7109375" customWidth="1"/>
+    <col min="44" max="44" width="11.7109375" customWidth="1"/>
+    <col min="45" max="45" width="9.42578125" customWidth="1"/>
+    <col min="46" max="46" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.28515625" style="1" customWidth="1"/>
     <col min="49" max="49" width="7" customWidth="1"/>
-    <col min="50" max="50" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="1.703125" customWidth="1"/>
-    <col min="52" max="52" width="11.64453125" customWidth="1"/>
-    <col min="53" max="53" width="9.41015625" customWidth="1"/>
-    <col min="54" max="54" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="7.29296875" style="1" customWidth="1"/>
+    <col min="50" max="50" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="1.7109375" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" customWidth="1"/>
+    <col min="53" max="53" width="9.42578125" customWidth="1"/>
+    <col min="54" max="54" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.28515625" style="1" customWidth="1"/>
     <col min="57" max="57" width="7" customWidth="1"/>
-    <col min="58" max="58" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="2.76171875" style="2" customWidth="1"/>
-    <col min="60" max="60" width="11.64453125" customWidth="1"/>
-    <col min="61" max="61" width="9.41015625" customWidth="1"/>
-    <col min="62" max="62" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.29296875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="2.7109375" style="2" customWidth="1"/>
+    <col min="60" max="60" width="11.7109375" customWidth="1"/>
+    <col min="61" max="61" width="9.42578125" customWidth="1"/>
+    <col min="62" max="62" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.28515625" style="1" customWidth="1"/>
     <col min="65" max="65" width="7" customWidth="1"/>
-    <col min="66" max="66" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="1.703125" customWidth="1"/>
-    <col min="68" max="68" width="11.64453125" customWidth="1"/>
-    <col min="69" max="69" width="9.41015625" customWidth="1"/>
-    <col min="70" max="70" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.29296875" style="1" customWidth="1"/>
+    <col min="66" max="66" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="1.7109375" customWidth="1"/>
+    <col min="68" max="68" width="11.7109375" customWidth="1"/>
+    <col min="69" max="69" width="9.42578125" customWidth="1"/>
+    <col min="70" max="70" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.28515625" style="1" customWidth="1"/>
     <col min="73" max="73" width="7" customWidth="1"/>
-    <col min="74" max="74" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="1.703125" customWidth="1"/>
-    <col min="76" max="76" width="11.64453125" customWidth="1"/>
-    <col min="77" max="77" width="9.41015625" customWidth="1"/>
-    <col min="78" max="78" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="7.29296875" style="1" customWidth="1"/>
+    <col min="74" max="74" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="1.7109375" customWidth="1"/>
+    <col min="76" max="76" width="11.7109375" customWidth="1"/>
+    <col min="77" max="77" width="9.42578125" customWidth="1"/>
+    <col min="78" max="78" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="7.28515625" style="1" customWidth="1"/>
     <col min="81" max="81" width="7" customWidth="1"/>
-    <col min="82" max="82" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="1.703125" customWidth="1"/>
-    <col min="84" max="84" width="11.64453125" customWidth="1"/>
-    <col min="85" max="85" width="9.41015625" customWidth="1"/>
-    <col min="86" max="86" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="7.29296875" style="1" customWidth="1"/>
+    <col min="82" max="82" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="1.7109375" customWidth="1"/>
+    <col min="84" max="84" width="11.7109375" customWidth="1"/>
+    <col min="85" max="85" width="9.42578125" customWidth="1"/>
+    <col min="86" max="86" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="7.28515625" style="1" customWidth="1"/>
     <col min="89" max="89" width="7" customWidth="1"/>
-    <col min="90" max="90" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="1.703125" customWidth="1"/>
-    <col min="92" max="92" width="11.64453125" customWidth="1"/>
-    <col min="93" max="93" width="9.41015625" customWidth="1"/>
-    <col min="94" max="94" width="7.29296875" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="7.29296875" style="1" customWidth="1"/>
+    <col min="90" max="90" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="1.7109375" customWidth="1"/>
+    <col min="92" max="92" width="11.7109375" customWidth="1"/>
+    <col min="93" max="93" width="9.42578125" customWidth="1"/>
+    <col min="94" max="94" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="7.28515625" style="1" customWidth="1"/>
     <col min="97" max="97" width="7" customWidth="1"/>
-    <col min="98" max="98" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="1.703125" customWidth="1"/>
+    <col min="98" max="98" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:99" x14ac:dyDescent="0.25">
       <c r="BG1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1590,7 +1595,7 @@
       <c r="CT2" s="3"/>
       <c r="CU2" s="3"/>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1714,7 +1719,7 @@
       <c r="CT3" s="5"/>
       <c r="CU3" s="3"/>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="7"/>
@@ -1874,7 +1879,7 @@
       </c>
       <c r="CU4" s="10"/>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2046,7 +2051,7 @@
       </c>
       <c r="CU5" s="10"/>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>44926</v>
       </c>
@@ -2172,7 +2177,7 @@
       <c r="CT6" s="15"/>
       <c r="CU6" s="16"/>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2288,7 +2293,7 @@
       <c r="CT7" s="17"/>
       <c r="CU7" s="17"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="18"/>
       <c r="C8" s="7"/>
@@ -2430,7 +2435,7 @@
       <c r="CT8" s="17"/>
       <c r="CU8" s="17"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>32</v>
       </c>
@@ -2590,7 +2595,7 @@
       <c r="CT9" s="29"/>
       <c r="CU9" s="10"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>34</v>
       </c>
@@ -2750,7 +2755,7 @@
       <c r="CT10" s="33"/>
       <c r="CU10" s="10"/>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>35</v>
       </c>
@@ -2896,7 +2901,7 @@
       <c r="CT11" s="33"/>
       <c r="CU11" s="10"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>36</v>
       </c>
@@ -3042,7 +3047,7 @@
       <c r="CT12" s="10"/>
       <c r="CU12" s="10"/>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>38</v>
       </c>
@@ -3188,7 +3193,7 @@
       <c r="CT13" s="10"/>
       <c r="CU13" s="10"/>
     </row>
-    <row r="14" spans="1:99" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:99" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="19" t="s">
         <v>39</v>
@@ -3329,7 +3334,7 @@
       <c r="CT14" s="10"/>
       <c r="CU14" s="10"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="C15" s="36"/>
       <c r="D15" s="37" t="s">
@@ -3457,7 +3462,7 @@
       <c r="CT15" s="40"/>
       <c r="CU15" s="41"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -3585,7 +3590,7 @@
       <c r="CT16" s="43"/>
       <c r="CU16" s="43"/>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>42</v>
       </c>
@@ -3711,7 +3716,7 @@
       <c r="CT17" s="14"/>
       <c r="CU17" s="16"/>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -3847,7 +3852,7 @@
       </c>
       <c r="CU18" s="10"/>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -4007,7 +4012,7 @@
       </c>
       <c r="CU19" s="10"/>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>32</v>
       </c>
@@ -4203,7 +4208,7 @@
       </c>
       <c r="CU20" s="10"/>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>34</v>
       </c>
@@ -4397,7 +4402,7 @@
       </c>
       <c r="CU21" s="10"/>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>35</v>
       </c>
@@ -4565,7 +4570,7 @@
       </c>
       <c r="CU22" s="10"/>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>36</v>
       </c>
@@ -4741,7 +4746,7 @@
       </c>
       <c r="CU23" s="10"/>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>38</v>
       </c>
@@ -4917,7 +4922,7 @@
       </c>
       <c r="CU24" s="10"/>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -5079,7 +5084,7 @@
       </c>
       <c r="CU25" s="10"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -5228,7 +5233,7 @@
       </c>
       <c r="CU26" s="41"/>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="24"/>
       <c r="C27" s="7"/>
@@ -5376,7 +5381,7 @@
       </c>
       <c r="CU27" s="43"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5465,7 +5470,7 @@
       <c r="CS28" s="3"/>
       <c r="CT28" s="3"/>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A29" s="46"/>
       <c r="B29" s="46"/>
       <c r="C29" s="47"/>
@@ -5709,7 +5714,7 @@
       </c>
       <c r="CU29" s="46"/>
     </row>
-    <row r="30" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50"/>
       <c r="B30" s="51"/>
       <c r="D30" s="50"/>
@@ -5816,7 +5821,7 @@
       <c r="CT30" s="53"/>
       <c r="CU30" s="53"/>
     </row>
-    <row r="31" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="50"/>
       <c r="B31" s="55"/>
       <c r="C31" s="56"/>
@@ -5924,7 +5929,7 @@
       <c r="CT31" s="31"/>
       <c r="CU31" s="53"/>
     </row>
-    <row r="32" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50"/>
       <c r="B32" s="50"/>
       <c r="D32" s="57"/>
@@ -6031,7 +6036,7 @@
       <c r="CT32" s="31"/>
       <c r="CU32" s="53"/>
     </row>
-    <row r="33" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50"/>
       <c r="B33" s="50"/>
       <c r="D33" s="57"/>
@@ -6138,7 +6143,7 @@
       <c r="CT33" s="31"/>
       <c r="CU33" s="53"/>
     </row>
-    <row r="34" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
       <c r="B34" s="50"/>
       <c r="D34" s="57"/>
@@ -6246,7 +6251,7 @@
       <c r="CT34" s="31"/>
       <c r="CU34" s="53"/>
     </row>
-    <row r="35" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
       <c r="C35" s="47"/>
       <c r="D35" s="61"/>
@@ -6353,7 +6358,7 @@
       <c r="CT35" s="63"/>
       <c r="CU35" s="65"/>
     </row>
-    <row r="36" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
       <c r="B36" s="51"/>
       <c r="D36" s="57"/>
@@ -6460,7 +6465,7 @@
       <c r="CT36" s="31"/>
       <c r="CU36" s="53"/>
     </row>
-    <row r="37" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:99" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
       <c r="B37" s="51"/>
       <c r="D37" s="57"/>
@@ -6567,7 +6572,7 @@
       <c r="CT37" s="31"/>
       <c r="CU37" s="53"/>
     </row>
-    <row r="38" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
       <c r="B38" s="51"/>
       <c r="C38"/>
@@ -6676,7 +6681,7 @@
       <c r="CT38" s="31"/>
       <c r="CU38" s="53"/>
     </row>
-    <row r="39" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="51"/>
       <c r="C39"/>
@@ -6785,7 +6790,7 @@
       <c r="CT39" s="31"/>
       <c r="CU39" s="53"/>
     </row>
-    <row r="40" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="50"/>
       <c r="B40" s="51"/>
       <c r="C40"/>
@@ -6894,7 +6899,7 @@
       <c r="CT40" s="31"/>
       <c r="CU40" s="53"/>
     </row>
-    <row r="41" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="50"/>
       <c r="B41" s="51"/>
       <c r="C41"/>
@@ -7003,7 +7008,7 @@
       <c r="CT41" s="31"/>
       <c r="CU41" s="53"/>
     </row>
-    <row r="42" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="50"/>
       <c r="B42" s="51"/>
       <c r="C42"/>
@@ -7112,7 +7117,7 @@
       <c r="CT42" s="31"/>
       <c r="CU42" s="53"/>
     </row>
-    <row r="43" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="50"/>
       <c r="B43" s="51"/>
       <c r="C43"/>
@@ -7221,7 +7226,7 @@
       <c r="CT43" s="31"/>
       <c r="CU43" s="53"/>
     </row>
-    <row r="44" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50"/>
       <c r="B44" s="51"/>
       <c r="C44"/>
@@ -7330,7 +7335,7 @@
       <c r="CT44" s="31"/>
       <c r="CU44" s="53"/>
     </row>
-    <row r="45" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="50"/>
       <c r="B45" s="51"/>
       <c r="C45"/>
@@ -7439,7 +7444,7 @@
       <c r="CT45" s="31"/>
       <c r="CU45" s="53"/>
     </row>
-    <row r="46" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="50"/>
       <c r="B46" s="51"/>
       <c r="C46"/>
@@ -7548,7 +7553,7 @@
       <c r="CT46" s="31"/>
       <c r="CU46" s="53"/>
     </row>
-    <row r="47" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="50"/>
       <c r="B47" s="51"/>
       <c r="C47"/>
@@ -7657,7 +7662,7 @@
       <c r="CT47" s="68"/>
       <c r="CU47" s="70"/>
     </row>
-    <row r="48" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="50"/>
       <c r="B48" s="51"/>
       <c r="C48"/>
@@ -7814,7 +7819,7 @@
       </c>
       <c r="CU48" s="65"/>
     </row>
-    <row r="49" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="50"/>
       <c r="B49" s="51"/>
       <c r="C49"/>
@@ -7971,7 +7976,7 @@
       </c>
       <c r="CU49" s="53"/>
     </row>
-    <row r="50" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="50"/>
       <c r="B50" s="51"/>
       <c r="C50"/>
@@ -8120,7 +8125,7 @@
       </c>
       <c r="CU50" s="53"/>
     </row>
-    <row r="51" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="50"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -8269,7 +8274,7 @@
       </c>
       <c r="CU51" s="53"/>
     </row>
-    <row r="52" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="50"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -8418,7 +8423,7 @@
       </c>
       <c r="CU52" s="53"/>
     </row>
-    <row r="53" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="50"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -8567,7 +8572,7 @@
       </c>
       <c r="CU53" s="53"/>
     </row>
-    <row r="54" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="50"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -8716,7 +8721,7 @@
       </c>
       <c r="CU54" s="53"/>
     </row>
-    <row r="55" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="50"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -8865,7 +8870,7 @@
       </c>
       <c r="CU55" s="53"/>
     </row>
-    <row r="56" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="50"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -9014,7 +9019,7 @@
       </c>
       <c r="CU56" s="53"/>
     </row>
-    <row r="57" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="50"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -9163,7 +9168,7 @@
       </c>
       <c r="CU57" s="53"/>
     </row>
-    <row r="58" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="50"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -9312,7 +9317,7 @@
       </c>
       <c r="CU58" s="53"/>
     </row>
-    <row r="59" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="50"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -9461,7 +9466,7 @@
       </c>
       <c r="CU59" s="70"/>
     </row>
-    <row r="60" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A60" s="50"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -9626,7 +9631,7 @@
       </c>
       <c r="CU60" s="53"/>
     </row>
-    <row r="61" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="50"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -9783,7 +9788,7 @@
       </c>
       <c r="CU61" s="53"/>
     </row>
-    <row r="62" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="50"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -9940,7 +9945,7 @@
       </c>
       <c r="CU62" s="53"/>
     </row>
-    <row r="63" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="50"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -10097,7 +10102,7 @@
       </c>
       <c r="CU63" s="53"/>
     </row>
-    <row r="64" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="50"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -10254,7 +10259,7 @@
       </c>
       <c r="CU64" s="53"/>
     </row>
-    <row r="65" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="50"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -10403,7 +10408,7 @@
       </c>
       <c r="CU65" s="53"/>
     </row>
-    <row r="66" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="50"/>
       <c r="B66"/>
       <c r="C66"/>
@@ -10552,7 +10557,7 @@
       </c>
       <c r="CU66" s="53"/>
     </row>
-    <row r="67" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="50"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -10701,7 +10706,7 @@
       </c>
       <c r="CU67" s="53"/>
     </row>
-    <row r="68" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="50"/>
       <c r="B68"/>
       <c r="C68"/>
@@ -10850,7 +10855,7 @@
       </c>
       <c r="CU68" s="53"/>
     </row>
-    <row r="69" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="50"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -10999,7 +11004,7 @@
       </c>
       <c r="CU69" s="53"/>
     </row>
-    <row r="70" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="50"/>
       <c r="B70"/>
       <c r="C70"/>
@@ -11140,7 +11145,7 @@
       </c>
       <c r="CU70" s="53"/>
     </row>
-    <row r="71" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="50"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -11281,7 +11286,7 @@
       </c>
       <c r="CU71" s="53"/>
     </row>
-    <row r="72" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="50"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -11422,7 +11427,7 @@
       </c>
       <c r="CU72" s="70"/>
     </row>
-    <row r="73" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A73" s="50"/>
       <c r="B73"/>
       <c r="C73"/>
@@ -11571,7 +11576,7 @@
       </c>
       <c r="CU73" s="53"/>
     </row>
-    <row r="74" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="50"/>
       <c r="B74"/>
       <c r="C74"/>
@@ -11720,7 +11725,7 @@
       </c>
       <c r="CU74" s="53"/>
     </row>
-    <row r="75" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="50"/>
       <c r="B75"/>
       <c r="C75"/>
@@ -11869,7 +11874,7 @@
       </c>
       <c r="CU75" s="53"/>
     </row>
-    <row r="76" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="50"/>
       <c r="B76"/>
       <c r="C76"/>
@@ -12018,7 +12023,7 @@
       </c>
       <c r="CU76" s="53"/>
     </row>
-    <row r="77" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="50"/>
       <c r="B77"/>
       <c r="C77"/>
@@ -12167,7 +12172,7 @@
       </c>
       <c r="CU77" s="53"/>
     </row>
-    <row r="78" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="50"/>
       <c r="B78"/>
       <c r="C78"/>
@@ -12316,7 +12321,7 @@
       </c>
       <c r="CU78" s="53"/>
     </row>
-    <row r="79" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="50"/>
       <c r="B79"/>
       <c r="C79"/>
@@ -12465,7 +12470,7 @@
       </c>
       <c r="CU79" s="53"/>
     </row>
-    <row r="80" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="50"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -12614,7 +12619,7 @@
       </c>
       <c r="CU80" s="53"/>
     </row>
-    <row r="81" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="50"/>
       <c r="B81"/>
       <c r="C81"/>
@@ -12763,7 +12768,7 @@
       </c>
       <c r="CU81" s="53"/>
     </row>
-    <row r="82" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="50"/>
       <c r="B82"/>
       <c r="C82"/>
@@ -12912,7 +12917,7 @@
       </c>
       <c r="CU82" s="53"/>
     </row>
-    <row r="83" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="50"/>
       <c r="B83"/>
       <c r="C83"/>
@@ -13061,7 +13066,7 @@
       </c>
       <c r="CU83" s="53"/>
     </row>
-    <row r="84" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="50"/>
       <c r="B84"/>
       <c r="C84"/>
@@ -13210,7 +13215,7 @@
       </c>
       <c r="CU84" s="53"/>
     </row>
-    <row r="85" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="50"/>
       <c r="B85"/>
       <c r="C85"/>
@@ -13359,7 +13364,7 @@
       </c>
       <c r="CU85" s="70"/>
     </row>
-    <row r="86" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A86" s="50"/>
       <c r="B86"/>
       <c r="C86"/>
@@ -13508,7 +13513,7 @@
       </c>
       <c r="CU86" s="53"/>
     </row>
-    <row r="87" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="50"/>
       <c r="B87"/>
       <c r="C87"/>
@@ -13657,7 +13662,7 @@
       </c>
       <c r="CU87" s="53"/>
     </row>
-    <row r="88" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="50"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -13798,7 +13803,7 @@
       <c r="CT88" s="31"/>
       <c r="CU88" s="53"/>
     </row>
-    <row r="89" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="50"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -13939,7 +13944,7 @@
       <c r="CT89" s="31"/>
       <c r="CU89" s="53"/>
     </row>
-    <row r="90" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="50"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -14080,7 +14085,7 @@
       <c r="CT90" s="31"/>
       <c r="CU90" s="53"/>
     </row>
-    <row r="91" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="50"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -14221,7 +14226,7 @@
       <c r="CT91" s="31"/>
       <c r="CU91" s="53"/>
     </row>
-    <row r="92" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="50"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -14362,7 +14367,7 @@
       <c r="CT92" s="31"/>
       <c r="CU92" s="53"/>
     </row>
-    <row r="93" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="50"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -14503,7 +14508,7 @@
       <c r="CT93" s="31"/>
       <c r="CU93" s="53"/>
     </row>
-    <row r="94" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="50"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -14644,7 +14649,7 @@
       <c r="CT94" s="31"/>
       <c r="CU94" s="53"/>
     </row>
-    <row r="95" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="50"/>
       <c r="B95"/>
       <c r="C95"/>
@@ -14785,7 +14790,7 @@
       <c r="CT95" s="31"/>
       <c r="CU95" s="53"/>
     </row>
-    <row r="96" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="50"/>
       <c r="B96"/>
       <c r="C96"/>
@@ -14926,7 +14931,7 @@
       <c r="CT96" s="31"/>
       <c r="CU96" s="53"/>
     </row>
-    <row r="97" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="50"/>
       <c r="B97"/>
       <c r="C97"/>
@@ -15067,7 +15072,7 @@
       <c r="CT97" s="31"/>
       <c r="CU97" s="53"/>
     </row>
-    <row r="98" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="50"/>
       <c r="B98"/>
       <c r="C98"/>
@@ -15176,7 +15181,7 @@
       <c r="CT98" s="31"/>
       <c r="CU98" s="70"/>
     </row>
-    <row r="99" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A99" s="50"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -15317,7 +15322,7 @@
       <c r="CT99" s="63"/>
       <c r="CU99" s="53"/>
     </row>
-    <row r="100" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="50"/>
       <c r="B100"/>
       <c r="C100"/>
@@ -15458,7 +15463,7 @@
       <c r="CT100" s="31"/>
       <c r="CU100" s="53"/>
     </row>
-    <row r="101" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="50"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -15599,7 +15604,7 @@
       <c r="CT101" s="31"/>
       <c r="CU101" s="53"/>
     </row>
-    <row r="102" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="50"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -15740,7 +15745,7 @@
       <c r="CT102" s="31"/>
       <c r="CU102" s="53"/>
     </row>
-    <row r="103" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="50"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -15881,7 +15886,7 @@
       <c r="CT103" s="31"/>
       <c r="CU103" s="53"/>
     </row>
-    <row r="104" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="50"/>
       <c r="B104"/>
       <c r="C104"/>
@@ -16022,7 +16027,7 @@
       <c r="CT104" s="31"/>
       <c r="CU104" s="53"/>
     </row>
-    <row r="105" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="50"/>
       <c r="B105"/>
       <c r="C105"/>
@@ -16163,7 +16168,7 @@
       <c r="CT105" s="31"/>
       <c r="CU105" s="53"/>
     </row>
-    <row r="106" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="50"/>
       <c r="B106"/>
       <c r="C106"/>
@@ -16304,7 +16309,7 @@
       <c r="CT106" s="31"/>
       <c r="CU106" s="53"/>
     </row>
-    <row r="107" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="50"/>
       <c r="B107"/>
       <c r="C107"/>
@@ -16445,7 +16450,7 @@
       <c r="CT107" s="31"/>
       <c r="CU107" s="53"/>
     </row>
-    <row r="108" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="50"/>
       <c r="B108"/>
       <c r="C108"/>
@@ -16586,7 +16591,7 @@
       <c r="CT108" s="31"/>
       <c r="CU108" s="53"/>
     </row>
-    <row r="109" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="50"/>
       <c r="B109"/>
       <c r="C109"/>
@@ -16727,7 +16732,7 @@
       <c r="CT109" s="31"/>
       <c r="CU109" s="53"/>
     </row>
-    <row r="110" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="50"/>
       <c r="B110"/>
       <c r="C110"/>
@@ -16868,7 +16873,7 @@
       <c r="CT110" s="68"/>
       <c r="CU110" s="70"/>
     </row>
-    <row r="111" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A111" s="50"/>
       <c r="B111"/>
       <c r="C111"/>
@@ -17009,7 +17014,7 @@
       <c r="CT111" s="31"/>
       <c r="CU111" s="53"/>
     </row>
-    <row r="112" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" s="50"/>
       <c r="B112"/>
       <c r="C112"/>
@@ -17150,7 +17155,7 @@
       <c r="CT112" s="31"/>
       <c r="CU112" s="53"/>
     </row>
-    <row r="113" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A113" s="50"/>
       <c r="B113"/>
       <c r="C113"/>
@@ -17291,7 +17296,7 @@
       <c r="CT113" s="31"/>
       <c r="CU113" s="53"/>
     </row>
-    <row r="114" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="50"/>
       <c r="B114"/>
       <c r="C114"/>
@@ -17432,7 +17437,7 @@
       <c r="CT114" s="31"/>
       <c r="CU114" s="53"/>
     </row>
-    <row r="115" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A115" s="50"/>
       <c r="B115"/>
       <c r="C115"/>
@@ -17573,7 +17578,7 @@
       <c r="CT115" s="31"/>
       <c r="CU115" s="53"/>
     </row>
-    <row r="116" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A116" s="50"/>
       <c r="B116"/>
       <c r="C116"/>
@@ -17714,7 +17719,7 @@
       <c r="CT116" s="31"/>
       <c r="CU116" s="53"/>
     </row>
-    <row r="117" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="50"/>
       <c r="B117"/>
       <c r="C117"/>
@@ -17855,7 +17860,7 @@
       <c r="CT117" s="31"/>
       <c r="CU117" s="53"/>
     </row>
-    <row r="118" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A118" s="50"/>
       <c r="B118"/>
       <c r="C118"/>
@@ -18012,7 +18017,7 @@
       <c r="CT118" s="31"/>
       <c r="CU118" s="53"/>
     </row>
-    <row r="119" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A119" s="50"/>
       <c r="B119"/>
       <c r="C119"/>
@@ -18149,7 +18154,7 @@
       <c r="CT119" s="31"/>
       <c r="CU119" s="53"/>
     </row>
-    <row r="120" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A120" s="50"/>
       <c r="B120"/>
       <c r="C120"/>
@@ -18298,7 +18303,7 @@
       <c r="CT120" s="31"/>
       <c r="CU120" s="53"/>
     </row>
-    <row r="121" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A121" s="50"/>
       <c r="B121"/>
       <c r="C121"/>
@@ -18447,7 +18452,7 @@
       <c r="CT121" s="31"/>
       <c r="CU121" s="53"/>
     </row>
-    <row r="122" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A122" s="50"/>
       <c r="B122"/>
       <c r="C122"/>
@@ -18596,7 +18601,7 @@
       <c r="CT122" s="31"/>
       <c r="CU122" s="53"/>
     </row>
-    <row r="123" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A123" s="50"/>
       <c r="B123"/>
       <c r="C123"/>
@@ -18745,7 +18750,7 @@
       <c r="CT123" s="31"/>
       <c r="CU123" s="53"/>
     </row>
-    <row r="124" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A124" s="50"/>
       <c r="B124"/>
       <c r="C124"/>
@@ -18894,7 +18899,7 @@
       <c r="CT124" s="31"/>
       <c r="CU124" s="70"/>
     </row>
-    <row r="125" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:99" s="47" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A125" s="50"/>
       <c r="B125"/>
       <c r="C125"/>
@@ -19043,7 +19048,7 @@
       <c r="CT125" s="63"/>
       <c r="CU125" s="53"/>
     </row>
-    <row r="126" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A126" s="50"/>
       <c r="B126"/>
       <c r="C126"/>
@@ -19192,7 +19197,7 @@
       <c r="CT126" s="31"/>
       <c r="CU126" s="53"/>
     </row>
-    <row r="127" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A127" s="50"/>
       <c r="B127"/>
       <c r="C127"/>
@@ -19341,7 +19346,7 @@
       <c r="CT127" s="31"/>
       <c r="CU127" s="53"/>
     </row>
-    <row r="128" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A128" s="50"/>
       <c r="B128"/>
       <c r="C128"/>
@@ -19490,7 +19495,7 @@
       <c r="CT128" s="31"/>
       <c r="CU128" s="53"/>
     </row>
-    <row r="129" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A129" s="50"/>
       <c r="B129"/>
       <c r="C129"/>
@@ -19639,7 +19644,7 @@
       <c r="CT129" s="31"/>
       <c r="CU129" s="53"/>
     </row>
-    <row r="130" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:99" s="47" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A130" s="50"/>
       <c r="B130"/>
       <c r="C130"/>
@@ -19788,7 +19793,7 @@
       <c r="CT130" s="68"/>
       <c r="CU130" s="70"/>
     </row>
-    <row r="131" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="50"/>
       <c r="B131"/>
       <c r="C131"/>
@@ -19889,7 +19894,7 @@
       <c r="CT131" s="31"/>
       <c r="CU131" s="53"/>
     </row>
-    <row r="132" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="50"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -19990,7 +19995,7 @@
       <c r="CT132" s="31"/>
       <c r="CU132" s="53"/>
     </row>
-    <row r="133" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133"/>
       <c r="B133"/>
       <c r="C133"/>
@@ -20089,7 +20094,7 @@
         <v>1.2759001117238278</v>
       </c>
       <c r="BZ133" s="31">
-        <v>4669.2514000000001</v>
+        <v>-4669.2514000000001</v>
       </c>
       <c r="CA133" s="58"/>
       <c r="CB133" s="31"/>
@@ -20121,7 +20126,7 @@
         <v>1.1213581264320203</v>
       </c>
       <c r="CP133" s="31">
-        <v>2263.7160999999996</v>
+        <v>-2263.7161000000001</v>
       </c>
       <c r="CQ133" s="58"/>
       <c r="CR133" s="31"/>
@@ -20131,7 +20136,7 @@
       </c>
       <c r="CU133" s="53"/>
     </row>
-    <row r="134" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="51"/>
       <c r="B134"/>
       <c r="C134"/>
@@ -20232,7 +20237,7 @@
       <c r="CT134" s="31"/>
       <c r="CU134"/>
     </row>
-    <row r="135" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="51"/>
       <c r="B135"/>
       <c r="C135"/>
@@ -20333,7 +20338,7 @@
       <c r="CT135" s="31"/>
       <c r="CU135"/>
     </row>
-    <row r="136" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="51"/>
       <c r="B136"/>
       <c r="C136"/>
@@ -20434,7 +20439,7 @@
       <c r="CT136" s="31"/>
       <c r="CU136"/>
     </row>
-    <row r="137" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="51"/>
       <c r="B137"/>
       <c r="C137"/>
@@ -20535,7 +20540,7 @@
       <c r="CT137" s="31"/>
       <c r="CU137" s="71"/>
     </row>
-    <row r="138" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="51"/>
       <c r="B138"/>
       <c r="C138"/>
@@ -20636,7 +20641,7 @@
       <c r="CT138" s="31"/>
       <c r="CU138" s="71"/>
     </row>
-    <row r="139" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="51"/>
       <c r="B139"/>
       <c r="C139"/>
@@ -20737,7 +20742,7 @@
       <c r="CT139" s="31"/>
       <c r="CU139" s="71"/>
     </row>
-    <row r="140" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="51"/>
       <c r="B140"/>
       <c r="C140"/>
@@ -20838,7 +20843,7 @@
       <c r="CT140" s="31"/>
       <c r="CU140" s="1"/>
     </row>
-    <row r="141" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="51"/>
       <c r="B141"/>
       <c r="C141"/>
@@ -20939,7 +20944,7 @@
       <c r="CT141"/>
       <c r="CU141" s="1"/>
     </row>
-    <row r="142" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="51"/>
       <c r="B142"/>
       <c r="C142"/>
@@ -21040,7 +21045,7 @@
       <c r="CT142"/>
       <c r="CU142" s="1"/>
     </row>
-    <row r="143" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="51"/>
       <c r="B143"/>
       <c r="C143"/>
@@ -21141,7 +21146,7 @@
       <c r="CT143"/>
       <c r="CU143"/>
     </row>
-    <row r="144" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:99" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="51"/>
       <c r="B144"/>
       <c r="C144"/>
@@ -21242,10 +21247,10 @@
       <c r="CT144"/>
       <c r="CU144"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="51"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="51"/>
     </row>
   </sheetData>

</xml_diff>